<commit_message>
Update data (rename no faculty to UtrechtUniversity)
</commit_message>
<xml_diff>
--- a/data/users_labeled.xlsx
+++ b/data/users_labeled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beld\Documents\GitHub\code-master-thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E12EF72-96D5-4DD1-8AFD-27A15E943FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EF187C-5E09-4179-9ADA-91161E324DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10618,13 +10618,13 @@
     <t>This is directly related to the chair of the professor so it's fine to keep the relation to him</t>
   </si>
   <si>
-    <t>No faculty</t>
-  </si>
-  <si>
     <t>employee_type</t>
   </si>
   <si>
     <t>Can still be retrieved by API but does not work at UU anymore. Faculty is changed manually</t>
+  </si>
+  <si>
+    <t>UtrechtUniversity</t>
   </si>
 </sst>
 </file>
@@ -11042,9 +11042,9 @@
   <dimension ref="A1:AV177"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="AV155" sqref="AV155"/>
+      <selection pane="bottomLeft" activeCell="AQ165" sqref="AQ165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11183,7 +11183,7 @@
         <v>40</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>3523</v>
+        <v>3522</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>41</v>
@@ -24163,7 +24163,7 @@
         <v>1</v>
       </c>
       <c r="AO104" t="s">
-        <v>3524</v>
+        <v>3523</v>
       </c>
       <c r="AP104" t="s">
         <v>2518</v>
@@ -31332,7 +31332,7 @@
         <v>2519</v>
       </c>
       <c r="AQ162" t="s">
-        <v>3522</v>
+        <v>3524</v>
       </c>
     </row>
     <row r="163" spans="1:48" x14ac:dyDescent="0.25">

</xml_diff>